<commit_message>
Add new routes and logics for user info page. Add new chat block.
</commit_message>
<xml_diff>
--- a/docs/Rating/Rating.xlsx
+++ b/docs/Rating/Rating.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="F1 OSR 2011" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>Pilots</t>
   </si>
@@ -140,12 +140,18 @@
   <si>
     <t>Rating</t>
   </si>
+  <si>
+    <t>12-Bel</t>
+  </si>
+  <si>
+    <t>Ilya Ivashchenko</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +171,15 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -294,7 +309,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
@@ -322,6 +337,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Акцент1" xfId="2" builtinId="32"/>
@@ -331,7 +350,19 @@
     <cellStyle name="Акцент5" xfId="4" builtinId="45"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <i/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -342,12 +373,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:C26" totalsRowShown="0">
-  <autoFilter ref="A1:C26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:C27" totalsRowShown="0">
+  <autoFilter ref="A1:C27"/>
+  <sortState ref="A2:C27">
+    <sortCondition descending="1" ref="B1:B27"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Position"/>
-    <tableColumn id="2" name="Pilots"/>
-    <tableColumn id="3" name="Rating"/>
+    <tableColumn id="2" name="Rating" dataDxfId="0"/>
+    <tableColumn id="3" name="Pilots" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -642,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AQ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5:W30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +736,9 @@
       <c r="L3" s="6">
         <v>9</v>
       </c>
-      <c r="M3" s="6"/>
+      <c r="M3" s="6">
+        <v>8</v>
+      </c>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
@@ -749,8 +785,8 @@
       <c r="L4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="8">
-        <v>12</v>
+      <c r="M4" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="N4" s="8">
         <v>13</v>
@@ -783,83 +819,83 @@
         <v>0</v>
       </c>
       <c r="X4" s="4" t="str">
-        <f>B4</f>
+        <f t="shared" ref="X4:AQ4" si="0">B4</f>
         <v>1-Aus</v>
       </c>
       <c r="Y4" s="4" t="str">
-        <f>C4</f>
+        <f t="shared" si="0"/>
         <v>2-Mal</v>
       </c>
       <c r="Z4" s="4" t="str">
-        <f>D4</f>
+        <f t="shared" si="0"/>
         <v>3-Chi</v>
       </c>
       <c r="AA4" s="4" t="str">
-        <f>E4</f>
+        <f t="shared" si="0"/>
         <v>4-Bah</v>
       </c>
       <c r="AB4" s="4" t="str">
-        <f>F4</f>
+        <f t="shared" si="0"/>
         <v>5-Spa</v>
       </c>
       <c r="AC4" s="4" t="str">
-        <f>G4</f>
+        <f t="shared" si="0"/>
         <v>6-Mon</v>
       </c>
       <c r="AD4" s="4" t="str">
-        <f>H4</f>
+        <f t="shared" si="0"/>
         <v>7-Can</v>
       </c>
       <c r="AE4" s="4" t="str">
-        <f>I4</f>
+        <f t="shared" si="0"/>
         <v>8-Eur</v>
       </c>
       <c r="AF4" s="4" t="str">
-        <f>J4</f>
+        <f t="shared" si="0"/>
         <v>9-Gbr</v>
       </c>
       <c r="AG4" s="4" t="str">
-        <f>K4</f>
+        <f t="shared" si="0"/>
         <v>10-Ger</v>
       </c>
       <c r="AH4" s="4" t="str">
-        <f>L4</f>
+        <f t="shared" si="0"/>
         <v>11-Hun</v>
       </c>
-      <c r="AI4" s="4">
-        <f>M4</f>
-        <v>12</v>
+      <c r="AI4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>12-Bel</v>
       </c>
       <c r="AJ4" s="4">
-        <f>N4</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="AK4" s="4">
-        <f>O4</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="AL4" s="4">
-        <f>P4</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="AM4" s="4">
-        <f>Q4</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="AN4" s="4">
-        <f>R4</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="AO4" s="4">
-        <f>S4</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="AP4" s="4">
-        <f>T4</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="AQ4" s="4">
-        <f>U4</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -890,91 +926,91 @@
       <c r="T5" s="9"/>
       <c r="U5" s="9"/>
       <c r="V5">
-        <f>SUM(X5:AN5)</f>
+        <f t="shared" ref="V5:V10" si="1">SUM(X5:AN5)</f>
         <v>8.0999999999999989E-2</v>
       </c>
       <c r="W5" s="5" t="str">
-        <f>A5</f>
+        <f t="shared" ref="W5:W30" si="2">A5</f>
         <v>Evgeny Peshkov</v>
       </c>
       <c r="X5">
-        <f>IF(B5&lt;&gt;"",(B$3/1000)*((B$3+1)-B5),0)</f>
+        <f t="shared" ref="X5:X32" si="3">IF(B5&lt;&gt;"",(B$3/1000)*((B$3+1)-B5),0)</f>
         <v>0</v>
       </c>
       <c r="Y5">
-        <f>IF(C5&lt;&gt;"",(C$3/1000)*((C$3+1)-C5),0)</f>
+        <f t="shared" ref="Y5:Y32" si="4">IF(C5&lt;&gt;"",(C$3/1000)*((C$3+1)-C5),0)</f>
         <v>0</v>
       </c>
       <c r="Z5">
-        <f>IF(D5&lt;&gt;"",(D$3/1000)*((D$3+1)-D5),0)</f>
+        <f t="shared" ref="Z5:Z32" si="5">IF(D5&lt;&gt;"",(D$3/1000)*((D$3+1)-D5),0)</f>
         <v>0</v>
       </c>
       <c r="AA5">
-        <f>IF(E5&lt;&gt;"",(E$3/1000)*((E$3+1)-E5),0)</f>
+        <f t="shared" ref="AA5:AA32" si="6">IF(E5&lt;&gt;"",(E$3/1000)*((E$3+1)-E5),0)</f>
         <v>0</v>
       </c>
       <c r="AB5">
-        <f>IF(F5&lt;&gt;"",(F$3/1000)*((F$3+1)-F5),0)</f>
+        <f t="shared" ref="AB5:AB32" si="7">IF(F5&lt;&gt;"",(F$3/1000)*((F$3+1)-F5),0)</f>
         <v>0</v>
       </c>
       <c r="AC5">
-        <f>IF(G5&lt;&gt;"",(G$3/1000)*((G$3+1)-G5),0)</f>
+        <f t="shared" ref="AC5:AC32" si="8">IF(G5&lt;&gt;"",(G$3/1000)*((G$3+1)-G5),0)</f>
         <v>0</v>
       </c>
       <c r="AD5">
-        <f>IF(H5&lt;&gt;"",(H$3/1000)*((H$3+1)-H5),0)</f>
+        <f t="shared" ref="AD5:AD32" si="9">IF(H5&lt;&gt;"",(H$3/1000)*((H$3+1)-H5),0)</f>
         <v>0</v>
       </c>
       <c r="AE5">
-        <f>IF(I5&lt;&gt;"",(I$3/1000)*((I$3+1)-I5),0)</f>
+        <f t="shared" ref="AE5:AE32" si="10">IF(I5&lt;&gt;"",(I$3/1000)*((I$3+1)-I5),0)</f>
         <v>0</v>
       </c>
       <c r="AF5">
-        <f>IF(J5&lt;&gt;"",(J$3/1000)*((J$3+1)-J5),0)</f>
+        <f t="shared" ref="AF5:AF32" si="11">IF(J5&lt;&gt;"",(J$3/1000)*((J$3+1)-J5),0)</f>
         <v>0</v>
       </c>
       <c r="AG5">
-        <f>IF(K5&lt;&gt;"",(K$3/1000)*((K$3+1)-K5),0)</f>
+        <f t="shared" ref="AG5:AG32" si="12">IF(K5&lt;&gt;"",(K$3/1000)*((K$3+1)-K5),0)</f>
         <v>8.0999999999999989E-2</v>
       </c>
       <c r="AH5">
-        <f>IF(L5&lt;&gt;"",(L$3/1000)*((L$3+1)-L5),0)</f>
+        <f t="shared" ref="AH5:AH32" si="13">IF(L5&lt;&gt;"",(L$3/1000)*((L$3+1)-L5),0)</f>
         <v>0</v>
       </c>
       <c r="AI5">
-        <f>IF(M5&lt;&gt;"",(M$3/1000)*((M$3+1)-M5),0)</f>
+        <f t="shared" ref="AI5:AI32" si="14">IF(M5&lt;&gt;"",(M$3/1000)*((M$3+1)-M5),0)</f>
         <v>0</v>
       </c>
       <c r="AJ5">
-        <f>IF(N5&lt;&gt;"",(N$3/1000)*((N$3+1)-N5),0)</f>
+        <f t="shared" ref="AJ5:AJ32" si="15">IF(N5&lt;&gt;"",(N$3/1000)*((N$3+1)-N5),0)</f>
         <v>0</v>
       </c>
       <c r="AK5">
-        <f>IF(O5&lt;&gt;"",(O$3/1000)*((O$3+1)-O5),0)</f>
+        <f t="shared" ref="AK5:AK32" si="16">IF(O5&lt;&gt;"",(O$3/1000)*((O$3+1)-O5),0)</f>
         <v>0</v>
       </c>
       <c r="AL5">
-        <f>IF(P5&lt;&gt;"",(P$3/1000)*((P$3+1)-P5),0)</f>
+        <f t="shared" ref="AL5:AL32" si="17">IF(P5&lt;&gt;"",(P$3/1000)*((P$3+1)-P5),0)</f>
         <v>0</v>
       </c>
       <c r="AM5">
-        <f>IF(Q5&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q5),0)</f>
+        <f t="shared" ref="AM5:AM32" si="18">IF(Q5&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q5),0)</f>
         <v>0</v>
       </c>
       <c r="AN5">
-        <f>IF(R5&lt;&gt;"",(R$3/1000)*((R$3+1)-R5),0)</f>
+        <f t="shared" ref="AN5:AN32" si="19">IF(R5&lt;&gt;"",(R$3/1000)*((R$3+1)-R5),0)</f>
         <v>0</v>
       </c>
       <c r="AO5">
-        <f>IF(S5&lt;&gt;"",(S$3/1000)*((S$3+1)-S5),0)</f>
+        <f t="shared" ref="AO5:AO32" si="20">IF(S5&lt;&gt;"",(S$3/1000)*((S$3+1)-S5),0)</f>
         <v>0</v>
       </c>
       <c r="AP5">
-        <f>IF(T5&lt;&gt;"",(T$3/1000)*((T$3+1)-T5),0)</f>
+        <f t="shared" ref="AP5:AP32" si="21">IF(T5&lt;&gt;"",(T$3/1000)*((T$3+1)-T5),0)</f>
         <v>0</v>
       </c>
       <c r="AQ5">
-        <f>IF(U5&lt;&gt;"",(U$3/1000)*((U$3+1)-U5),0)</f>
+        <f t="shared" ref="AQ5:AQ32" si="22">IF(U5&lt;&gt;"",(U$3/1000)*((U$3+1)-U5),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1015,7 +1051,9 @@
       <c r="L6" s="9">
         <v>1</v>
       </c>
-      <c r="M6" s="9"/>
+      <c r="M6" s="9">
+        <v>1</v>
+      </c>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
@@ -1025,91 +1063,91 @@
       <c r="T6" s="9"/>
       <c r="U6" s="9"/>
       <c r="V6">
-        <f>SUM(X6:AN6)</f>
-        <v>0.78999999999999992</v>
+        <f t="shared" si="1"/>
+        <v>0.85399999999999987</v>
       </c>
       <c r="W6" s="5" t="str">
-        <f>A6</f>
+        <f t="shared" si="2"/>
         <v>Evgeny Egorenko</v>
       </c>
       <c r="X6">
-        <f>IF(B6&lt;&gt;"",(B$3/1000)*((B$3+1)-B6),0)</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="Y6">
-        <f>IF(C6&lt;&gt;"",(C$3/1000)*((C$3+1)-C6),0)</f>
+        <f t="shared" si="4"/>
         <v>3.6000000000000004E-2</v>
       </c>
       <c r="Z6">
-        <f>IF(D6&lt;&gt;"",(D$3/1000)*((D$3+1)-D6),0)</f>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="AA6">
-        <f>IF(E6&lt;&gt;"",(E$3/1000)*((E$3+1)-E6),0)</f>
+        <f t="shared" si="6"/>
         <v>8.0999999999999989E-2</v>
       </c>
       <c r="AB6">
-        <f>IF(F6&lt;&gt;"",(F$3/1000)*((F$3+1)-F6),0)</f>
+        <f t="shared" si="7"/>
         <v>3.6000000000000004E-2</v>
       </c>
       <c r="AC6">
-        <f>IF(G6&lt;&gt;"",(G$3/1000)*((G$3+1)-G6),0)</f>
+        <f t="shared" si="8"/>
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="AD6">
-        <f>IF(H6&lt;&gt;"",(H$3/1000)*((H$3+1)-H6),0)</f>
+        <f t="shared" si="9"/>
         <v>0.09</v>
       </c>
       <c r="AE6">
-        <f>IF(I6&lt;&gt;"",(I$3/1000)*((I$3+1)-I6),0)</f>
+        <f t="shared" si="10"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="AF6">
-        <f>IF(J6&lt;&gt;"",(J$3/1000)*((J$3+1)-J6),0)</f>
+        <f t="shared" si="11"/>
         <v>8.0999999999999989E-2</v>
       </c>
       <c r="AG6">
-        <f>IF(K6&lt;&gt;"",(K$3/1000)*((K$3+1)-K6),0)</f>
+        <f t="shared" si="12"/>
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="AH6">
-        <f>IF(L6&lt;&gt;"",(L$3/1000)*((L$3+1)-L6),0)</f>
+        <f t="shared" si="13"/>
         <v>8.0999999999999989E-2</v>
       </c>
       <c r="AI6">
-        <f>IF(M6&lt;&gt;"",(M$3/1000)*((M$3+1)-M6),0)</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AJ6">
-        <f>IF(N6&lt;&gt;"",(N$3/1000)*((N$3+1)-N6),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK6">
-        <f>IF(O6&lt;&gt;"",(O$3/1000)*((O$3+1)-O6),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL6">
-        <f>IF(P6&lt;&gt;"",(P$3/1000)*((P$3+1)-P6),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM6">
-        <f>IF(Q6&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q6),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN6">
-        <f>IF(R6&lt;&gt;"",(R$3/1000)*((R$3+1)-R6),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO6">
-        <f>IF(S6&lt;&gt;"",(S$3/1000)*((S$3+1)-S6),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP6">
-        <f>IF(T6&lt;&gt;"",(T$3/1000)*((T$3+1)-T6),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ6">
-        <f>IF(U6&lt;&gt;"",(U$3/1000)*((U$3+1)-U6),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -1140,91 +1178,91 @@
       <c r="T7" s="9"/>
       <c r="U7" s="9"/>
       <c r="V7">
-        <f>SUM(X7:AN7)</f>
+        <f t="shared" si="1"/>
         <v>6.3E-2</v>
       </c>
       <c r="W7" s="5" t="str">
-        <f>A7</f>
+        <f t="shared" si="2"/>
         <v>Sergey Lozgachev</v>
       </c>
       <c r="X7">
-        <f>IF(B7&lt;&gt;"",(B$3/1000)*((B$3+1)-B7),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y7">
-        <f>IF(C7&lt;&gt;"",(C$3/1000)*((C$3+1)-C7),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z7">
-        <f>IF(D7&lt;&gt;"",(D$3/1000)*((D$3+1)-D7),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA7">
-        <f>IF(E7&lt;&gt;"",(E$3/1000)*((E$3+1)-E7),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB7">
-        <f>IF(F7&lt;&gt;"",(F$3/1000)*((F$3+1)-F7),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC7">
-        <f>IF(G7&lt;&gt;"",(G$3/1000)*((G$3+1)-G7),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD7">
-        <f>IF(H7&lt;&gt;"",(H$3/1000)*((H$3+1)-H7),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE7">
-        <f>IF(I7&lt;&gt;"",(I$3/1000)*((I$3+1)-I7),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF7">
-        <f>IF(J7&lt;&gt;"",(J$3/1000)*((J$3+1)-J7),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG7">
-        <f>IF(K7&lt;&gt;"",(K$3/1000)*((K$3+1)-K7),0)</f>
+        <f t="shared" si="12"/>
         <v>6.3E-2</v>
       </c>
       <c r="AH7">
-        <f>IF(L7&lt;&gt;"",(L$3/1000)*((L$3+1)-L7),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI7">
-        <f>IF(M7&lt;&gt;"",(M$3/1000)*((M$3+1)-M7),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ7">
-        <f>IF(N7&lt;&gt;"",(N$3/1000)*((N$3+1)-N7),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK7">
-        <f>IF(O7&lt;&gt;"",(O$3/1000)*((O$3+1)-O7),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL7">
-        <f>IF(P7&lt;&gt;"",(P$3/1000)*((P$3+1)-P7),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM7">
-        <f>IF(Q7&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q7),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN7">
-        <f>IF(R7&lt;&gt;"",(R$3/1000)*((R$3+1)-R7),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO7">
-        <f>IF(S7&lt;&gt;"",(S$3/1000)*((S$3+1)-S7),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP7">
-        <f>IF(T7&lt;&gt;"",(T$3/1000)*((T$3+1)-T7),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ7">
-        <f>IF(U7&lt;&gt;"",(U$3/1000)*((U$3+1)-U7),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -1249,7 +1287,9 @@
       <c r="L8" s="9">
         <v>5</v>
       </c>
-      <c r="M8" s="9"/>
+      <c r="M8" s="9">
+        <v>2</v>
+      </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
@@ -1259,91 +1299,91 @@
       <c r="T8" s="9"/>
       <c r="U8" s="9"/>
       <c r="V8">
-        <f>SUM(X8:AN8)</f>
-        <v>0.16199999999999998</v>
+        <f t="shared" si="1"/>
+        <v>0.21799999999999997</v>
       </c>
       <c r="W8" s="5" t="str">
-        <f>A8</f>
+        <f t="shared" si="2"/>
         <v>Ivan Egorov</v>
       </c>
       <c r="X8">
-        <f>IF(B8&lt;&gt;"",(B$3/1000)*((B$3+1)-B8),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y8">
-        <f>IF(C8&lt;&gt;"",(C$3/1000)*((C$3+1)-C8),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z8">
-        <f>IF(D8&lt;&gt;"",(D$3/1000)*((D$3+1)-D8),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA8">
-        <f>IF(E8&lt;&gt;"",(E$3/1000)*((E$3+1)-E8),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB8">
-        <f>IF(F8&lt;&gt;"",(F$3/1000)*((F$3+1)-F8),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC8">
-        <f>IF(G8&lt;&gt;"",(G$3/1000)*((G$3+1)-G8),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD8">
-        <f>IF(H8&lt;&gt;"",(H$3/1000)*((H$3+1)-H8),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE8">
-        <f>IF(I8&lt;&gt;"",(I$3/1000)*((I$3+1)-I8),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF8">
-        <f>IF(J8&lt;&gt;"",(J$3/1000)*((J$3+1)-J8),0)</f>
+        <f t="shared" si="11"/>
         <v>6.3E-2</v>
       </c>
       <c r="AG8">
-        <f>IF(K8&lt;&gt;"",(K$3/1000)*((K$3+1)-K8),0)</f>
+        <f t="shared" si="12"/>
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="AH8">
-        <f>IF(L8&lt;&gt;"",(L$3/1000)*((L$3+1)-L8),0)</f>
+        <f t="shared" si="13"/>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="AI8">
-        <f>IF(M8&lt;&gt;"",(M$3/1000)*((M$3+1)-M8),0)</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="AJ8">
-        <f>IF(N8&lt;&gt;"",(N$3/1000)*((N$3+1)-N8),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK8">
-        <f>IF(O8&lt;&gt;"",(O$3/1000)*((O$3+1)-O8),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL8">
-        <f>IF(P8&lt;&gt;"",(P$3/1000)*((P$3+1)-P8),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM8">
-        <f>IF(Q8&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q8),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN8">
-        <f>IF(R8&lt;&gt;"",(R$3/1000)*((R$3+1)-R8),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO8">
-        <f>IF(S8&lt;&gt;"",(S$3/1000)*((S$3+1)-S8),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP8">
-        <f>IF(T8&lt;&gt;"",(T$3/1000)*((T$3+1)-T8),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ8">
-        <f>IF(U8&lt;&gt;"",(U$3/1000)*((U$3+1)-U8),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -1366,7 +1406,9 @@
       <c r="L9" s="9">
         <v>3</v>
       </c>
-      <c r="M9" s="9"/>
+      <c r="M9" s="9">
+        <v>8</v>
+      </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
@@ -1376,91 +1418,91 @@
       <c r="T9" s="9"/>
       <c r="U9" s="9"/>
       <c r="V9">
-        <f>SUM(X9:AN9)</f>
-        <v>0.108</v>
+        <f t="shared" si="1"/>
+        <v>0.11599999999999999</v>
       </c>
       <c r="W9" s="5" t="str">
-        <f>A9</f>
+        <f t="shared" si="2"/>
         <v>Ilya Alexandrov</v>
       </c>
       <c r="X9">
-        <f>IF(B9&lt;&gt;"",(B$3/1000)*((B$3+1)-B9),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y9">
-        <f>IF(C9&lt;&gt;"",(C$3/1000)*((C$3+1)-C9),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z9">
-        <f>IF(D9&lt;&gt;"",(D$3/1000)*((D$3+1)-D9),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA9">
-        <f>IF(E9&lt;&gt;"",(E$3/1000)*((E$3+1)-E9),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB9">
-        <f>IF(F9&lt;&gt;"",(F$3/1000)*((F$3+1)-F9),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC9">
-        <f>IF(G9&lt;&gt;"",(G$3/1000)*((G$3+1)-G9),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD9">
-        <f>IF(H9&lt;&gt;"",(H$3/1000)*((H$3+1)-H9),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE9">
-        <f>IF(I9&lt;&gt;"",(I$3/1000)*((I$3+1)-I9),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF9">
-        <f>IF(J9&lt;&gt;"",(J$3/1000)*((J$3+1)-J9),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG9">
-        <f>IF(K9&lt;&gt;"",(K$3/1000)*((K$3+1)-K9),0)</f>
+        <f t="shared" si="12"/>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="AH9">
-        <f>IF(L9&lt;&gt;"",(L$3/1000)*((L$3+1)-L9),0)</f>
+        <f t="shared" si="13"/>
         <v>6.3E-2</v>
       </c>
       <c r="AI9">
-        <f>IF(M9&lt;&gt;"",(M$3/1000)*((M$3+1)-M9),0)</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AJ9">
-        <f>IF(N9&lt;&gt;"",(N$3/1000)*((N$3+1)-N9),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK9">
-        <f>IF(O9&lt;&gt;"",(O$3/1000)*((O$3+1)-O9),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL9">
-        <f>IF(P9&lt;&gt;"",(P$3/1000)*((P$3+1)-P9),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM9">
-        <f>IF(Q9&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q9),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN9">
-        <f>IF(R9&lt;&gt;"",(R$3/1000)*((R$3+1)-R9),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO9">
-        <f>IF(S9&lt;&gt;"",(S$3/1000)*((S$3+1)-S9),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP9">
-        <f>IF(T9&lt;&gt;"",(T$3/1000)*((T$3+1)-T9),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ9">
-        <f>IF(U9&lt;&gt;"",(U$3/1000)*((U$3+1)-U9),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -1495,7 +1537,9 @@
       <c r="L10" s="9">
         <v>7</v>
       </c>
-      <c r="M10" s="9"/>
+      <c r="M10" s="9">
+        <v>5</v>
+      </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
@@ -1505,91 +1549,91 @@
       <c r="T10" s="9"/>
       <c r="U10" s="9"/>
       <c r="V10">
-        <f>SUM(X10:AN10)</f>
-        <v>0.32099999999999995</v>
+        <f t="shared" si="1"/>
+        <v>0.35299999999999998</v>
       </c>
       <c r="W10" s="5" t="str">
-        <f>A10</f>
+        <f t="shared" si="2"/>
         <v>Igor Peshkov</v>
       </c>
       <c r="X10">
-        <f>IF(B10&lt;&gt;"",(B$3/1000)*((B$3+1)-B10),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y10">
-        <f>IF(C10&lt;&gt;"",(C$3/1000)*((C$3+1)-C10),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z10">
-        <f>IF(D10&lt;&gt;"",(D$3/1000)*((D$3+1)-D10),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA10">
-        <f>IF(E10&lt;&gt;"",(E$3/1000)*((E$3+1)-E10),0)</f>
+        <f t="shared" si="6"/>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="AB10">
-        <f>IF(F10&lt;&gt;"",(F$3/1000)*((F$3+1)-F10),0)</f>
+        <f t="shared" si="7"/>
         <v>1.8000000000000002E-2</v>
       </c>
       <c r="AC10">
-        <f>IF(G10&lt;&gt;"",(G$3/1000)*((G$3+1)-G10),0)</f>
+        <f t="shared" si="8"/>
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="AD10">
-        <f>IF(H10&lt;&gt;"",(H$3/1000)*((H$3+1)-H10),0)</f>
+        <f t="shared" si="9"/>
         <v>0.1</v>
       </c>
       <c r="AE10">
-        <f>IF(I10&lt;&gt;"",(I$3/1000)*((I$3+1)-I10),0)</f>
+        <f t="shared" si="10"/>
         <v>1.6E-2</v>
       </c>
       <c r="AF10">
-        <f>IF(J10&lt;&gt;"",(J$3/1000)*((J$3+1)-J10),0)</f>
+        <f t="shared" si="11"/>
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="AG10">
-        <f>IF(K10&lt;&gt;"",(K$3/1000)*((K$3+1)-K10),0)</f>
+        <f t="shared" si="12"/>
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="AH10">
-        <f>IF(L10&lt;&gt;"",(L$3/1000)*((L$3+1)-L10),0)</f>
+        <f t="shared" si="13"/>
         <v>2.6999999999999996E-2</v>
       </c>
       <c r="AI10">
-        <f>IF(M10&lt;&gt;"",(M$3/1000)*((M$3+1)-M10),0)</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="AJ10">
-        <f>IF(N10&lt;&gt;"",(N$3/1000)*((N$3+1)-N10),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK10">
-        <f>IF(O10&lt;&gt;"",(O$3/1000)*((O$3+1)-O10),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL10">
-        <f>IF(P10&lt;&gt;"",(P$3/1000)*((P$3+1)-P10),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM10">
-        <f>IF(Q10&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q10),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN10">
-        <f>IF(R10&lt;&gt;"",(R$3/1000)*((R$3+1)-R10),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO10">
-        <f>IF(S10&lt;&gt;"",(S$3/1000)*((S$3+1)-S10),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP10">
-        <f>IF(T10&lt;&gt;"",(T$3/1000)*((T$3+1)-T10),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ10">
-        <f>IF(U10&lt;&gt;"",(U$3/1000)*((U$3+1)-U10),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -1636,91 +1680,91 @@
       <c r="T11" s="9"/>
       <c r="U11" s="9"/>
       <c r="V11">
-        <f t="shared" ref="V11:V21" si="0">SUM(X11:AN11)</f>
+        <f t="shared" ref="V11:V21" si="23">SUM(X11:AN11)</f>
         <v>0.35599999999999998</v>
       </c>
       <c r="W11" s="5" t="str">
-        <f>A11</f>
+        <f t="shared" si="2"/>
         <v>Andrey Vinokurov</v>
       </c>
       <c r="X11">
-        <f>IF(B11&lt;&gt;"",(B$3/1000)*((B$3+1)-B11),0)</f>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
       <c r="Y11">
-        <f>IF(C11&lt;&gt;"",(C$3/1000)*((C$3+1)-C11),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z11">
-        <f>IF(D11&lt;&gt;"",(D$3/1000)*((D$3+1)-D11),0)</f>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="AA11">
-        <f>IF(E11&lt;&gt;"",(E$3/1000)*((E$3+1)-E11),0)</f>
+        <f t="shared" si="6"/>
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="AB11">
-        <f>IF(F11&lt;&gt;"",(F$3/1000)*((F$3+1)-F11),0)</f>
+        <f t="shared" si="7"/>
         <v>1.2E-2</v>
       </c>
       <c r="AC11">
-        <f>IF(G11&lt;&gt;"",(G$3/1000)*((G$3+1)-G11),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD11">
-        <f>IF(H11&lt;&gt;"",(H$3/1000)*((H$3+1)-H11),0)</f>
+        <f t="shared" si="9"/>
         <v>0.04</v>
       </c>
       <c r="AE11">
-        <f>IF(I11&lt;&gt;"",(I$3/1000)*((I$3+1)-I11),0)</f>
+        <f t="shared" si="10"/>
         <v>0.04</v>
       </c>
       <c r="AF11">
-        <f>IF(J11&lt;&gt;"",(J$3/1000)*((J$3+1)-J11),0)</f>
+        <f t="shared" si="11"/>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="AG11">
-        <f>IF(K11&lt;&gt;"",(K$3/1000)*((K$3+1)-K11),0)</f>
+        <f t="shared" si="12"/>
         <v>2.6999999999999996E-2</v>
       </c>
       <c r="AH11">
-        <f>IF(L11&lt;&gt;"",(L$3/1000)*((L$3+1)-L11),0)</f>
+        <f t="shared" si="13"/>
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="AI11">
-        <f>IF(M11&lt;&gt;"",(M$3/1000)*((M$3+1)-M11),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ11">
-        <f>IF(N11&lt;&gt;"",(N$3/1000)*((N$3+1)-N11),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK11">
-        <f>IF(O11&lt;&gt;"",(O$3/1000)*((O$3+1)-O11),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL11">
-        <f>IF(P11&lt;&gt;"",(P$3/1000)*((P$3+1)-P11),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM11">
-        <f>IF(Q11&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q11),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN11">
-        <f>IF(R11&lt;&gt;"",(R$3/1000)*((R$3+1)-R11),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO11">
-        <f>IF(S11&lt;&gt;"",(S$3/1000)*((S$3+1)-S11),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP11">
-        <f>IF(T11&lt;&gt;"",(T$3/1000)*((T$3+1)-T11),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ11">
-        <f>IF(U11&lt;&gt;"",(U$3/1000)*((U$3+1)-U11),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -1751,7 +1795,9 @@
       <c r="L12" s="9">
         <v>9</v>
       </c>
-      <c r="M12" s="9"/>
+      <c r="M12" s="9">
+        <v>4</v>
+      </c>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
@@ -1761,91 +1807,91 @@
       <c r="T12" s="9"/>
       <c r="U12" s="9"/>
       <c r="V12">
-        <f t="shared" si="0"/>
-        <v>0.126</v>
+        <f t="shared" si="23"/>
+        <v>0.16600000000000001</v>
       </c>
       <c r="W12" s="5" t="str">
-        <f>A12</f>
+        <f t="shared" si="2"/>
         <v>Andrey Stasiukevich</v>
       </c>
       <c r="X12">
-        <f>IF(B12&lt;&gt;"",(B$3/1000)*((B$3+1)-B12),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y12">
-        <f>IF(C12&lt;&gt;"",(C$3/1000)*((C$3+1)-C12),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z12">
-        <f>IF(D12&lt;&gt;"",(D$3/1000)*((D$3+1)-D12),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA12">
-        <f>IF(E12&lt;&gt;"",(E$3/1000)*((E$3+1)-E12),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB12">
-        <f>IF(F12&lt;&gt;"",(F$3/1000)*((F$3+1)-F12),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC12">
-        <f>IF(G12&lt;&gt;"",(G$3/1000)*((G$3+1)-G12),0)</f>
+        <f t="shared" si="8"/>
         <v>1.4E-2</v>
       </c>
       <c r="AD12">
-        <f>IF(H12&lt;&gt;"",(H$3/1000)*((H$3+1)-H12),0)</f>
+        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
       <c r="AE12">
-        <f>IF(I12&lt;&gt;"",(I$3/1000)*((I$3+1)-I12),0)</f>
+        <f t="shared" si="10"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="AF12">
-        <f>IF(J12&lt;&gt;"",(J$3/1000)*((J$3+1)-J12),0)</f>
+        <f t="shared" si="11"/>
         <v>2.6999999999999996E-2</v>
       </c>
       <c r="AG12">
-        <f>IF(K12&lt;&gt;"",(K$3/1000)*((K$3+1)-K12),0)</f>
+        <f t="shared" si="12"/>
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="AH12">
-        <f>IF(L12&lt;&gt;"",(L$3/1000)*((L$3+1)-L12),0)</f>
+        <f t="shared" si="13"/>
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="AI12">
-        <f>IF(M12&lt;&gt;"",(M$3/1000)*((M$3+1)-M12),0)</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.04</v>
       </c>
       <c r="AJ12">
-        <f>IF(N12&lt;&gt;"",(N$3/1000)*((N$3+1)-N12),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK12">
-        <f>IF(O12&lt;&gt;"",(O$3/1000)*((O$3+1)-O12),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL12">
-        <f>IF(P12&lt;&gt;"",(P$3/1000)*((P$3+1)-P12),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM12">
-        <f>IF(Q12&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q12),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN12">
-        <f>IF(R12&lt;&gt;"",(R$3/1000)*((R$3+1)-R12),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO12">
-        <f>IF(S12&lt;&gt;"",(S$3/1000)*((S$3+1)-S12),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP12">
-        <f>IF(T12&lt;&gt;"",(T$3/1000)*((T$3+1)-T12),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ12">
-        <f>IF(U12&lt;&gt;"",(U$3/1000)*((U$3+1)-U12),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -1882,7 +1928,9 @@
       <c r="L13" s="9">
         <v>6</v>
       </c>
-      <c r="M13" s="9"/>
+      <c r="M13" s="9">
+        <v>6</v>
+      </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
@@ -1892,91 +1940,91 @@
       <c r="T13" s="9"/>
       <c r="U13" s="9"/>
       <c r="V13">
-        <f t="shared" si="0"/>
-        <v>0.30399999999999999</v>
+        <f t="shared" si="23"/>
+        <v>0.32800000000000001</v>
       </c>
       <c r="W13" s="5" t="str">
-        <f>A13</f>
+        <f t="shared" si="2"/>
         <v>Maksim Prokoshun</v>
       </c>
       <c r="X13">
-        <f>IF(B13&lt;&gt;"",(B$3/1000)*((B$3+1)-B13),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y13">
-        <f>IF(C13&lt;&gt;"",(C$3/1000)*((C$3+1)-C13),0)</f>
+        <f t="shared" si="4"/>
         <v>1.8000000000000002E-2</v>
       </c>
       <c r="Z13">
-        <f>IF(D13&lt;&gt;"",(D$3/1000)*((D$3+1)-D13),0)</f>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="AA13">
-        <f>IF(E13&lt;&gt;"",(E$3/1000)*((E$3+1)-E13),0)</f>
+        <f t="shared" si="6"/>
         <v>2.6999999999999996E-2</v>
       </c>
       <c r="AB13">
-        <f>IF(F13&lt;&gt;"",(F$3/1000)*((F$3+1)-F13),0)</f>
+        <f t="shared" si="7"/>
         <v>2.4E-2</v>
       </c>
       <c r="AC13">
-        <f>IF(G13&lt;&gt;"",(G$3/1000)*((G$3+1)-G13),0)</f>
+        <f t="shared" si="8"/>
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="AD13">
-        <f>IF(H13&lt;&gt;"",(H$3/1000)*((H$3+1)-H13),0)</f>
+        <f t="shared" si="9"/>
         <v>0.06</v>
       </c>
       <c r="AE13">
-        <f>IF(I13&lt;&gt;"",(I$3/1000)*((I$3+1)-I13),0)</f>
+        <f t="shared" si="10"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="AF13">
-        <f>IF(J13&lt;&gt;"",(J$3/1000)*((J$3+1)-J13),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f>IF(K13&lt;&gt;"",(K$3/1000)*((K$3+1)-K13),0)</f>
+        <f t="shared" si="12"/>
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="AH13">
-        <f>IF(L13&lt;&gt;"",(L$3/1000)*((L$3+1)-L13),0)</f>
+        <f t="shared" si="13"/>
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="AI13">
-        <f>IF(M13&lt;&gt;"",(M$3/1000)*((M$3+1)-M13),0)</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>2.4E-2</v>
       </c>
       <c r="AJ13">
-        <f>IF(N13&lt;&gt;"",(N$3/1000)*((N$3+1)-N13),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK13">
-        <f>IF(O13&lt;&gt;"",(O$3/1000)*((O$3+1)-O13),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL13">
-        <f>IF(P13&lt;&gt;"",(P$3/1000)*((P$3+1)-P13),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM13">
-        <f>IF(Q13&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q13),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN13">
-        <f>IF(R13&lt;&gt;"",(R$3/1000)*((R$3+1)-R13),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO13">
-        <f>IF(S13&lt;&gt;"",(S$3/1000)*((S$3+1)-S13),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP13">
-        <f>IF(T13&lt;&gt;"",(T$3/1000)*((T$3+1)-T13),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ13">
-        <f>IF(U13&lt;&gt;"",(U$3/1000)*((U$3+1)-U13),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -2007,91 +2055,91 @@
       <c r="T14" s="9"/>
       <c r="U14" s="9"/>
       <c r="V14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="23"/>
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="W14" s="5" t="str">
-        <f>A14</f>
+        <f t="shared" si="2"/>
         <v>Vadim Vrenere</v>
       </c>
       <c r="X14">
-        <f>IF(B14&lt;&gt;"",(B$3/1000)*((B$3+1)-B14),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y14">
-        <f>IF(C14&lt;&gt;"",(C$3/1000)*((C$3+1)-C14),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z14">
-        <f>IF(D14&lt;&gt;"",(D$3/1000)*((D$3+1)-D14),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA14">
-        <f>IF(E14&lt;&gt;"",(E$3/1000)*((E$3+1)-E14),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB14">
-        <f>IF(F14&lt;&gt;"",(F$3/1000)*((F$3+1)-F14),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC14">
-        <f>IF(G14&lt;&gt;"",(G$3/1000)*((G$3+1)-G14),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD14">
-        <f>IF(H14&lt;&gt;"",(H$3/1000)*((H$3+1)-H14),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE14">
-        <f>IF(I14&lt;&gt;"",(I$3/1000)*((I$3+1)-I14),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF14">
-        <f>IF(J14&lt;&gt;"",(J$3/1000)*((J$3+1)-J14),0)</f>
+        <f t="shared" si="11"/>
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="AG14">
-        <f>IF(K14&lt;&gt;"",(K$3/1000)*((K$3+1)-K14),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH14">
-        <f>IF(L14&lt;&gt;"",(L$3/1000)*((L$3+1)-L14),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI14">
-        <f>IF(M14&lt;&gt;"",(M$3/1000)*((M$3+1)-M14),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ14">
-        <f>IF(N14&lt;&gt;"",(N$3/1000)*((N$3+1)-N14),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK14">
-        <f>IF(O14&lt;&gt;"",(O$3/1000)*((O$3+1)-O14),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL14">
-        <f>IF(P14&lt;&gt;"",(P$3/1000)*((P$3+1)-P14),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM14">
-        <f>IF(Q14&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q14),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN14">
-        <f>IF(R14&lt;&gt;"",(R$3/1000)*((R$3+1)-R14),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO14">
-        <f>IF(S14&lt;&gt;"",(S$3/1000)*((S$3+1)-S14),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP14">
-        <f>IF(T14&lt;&gt;"",(T$3/1000)*((T$3+1)-T14),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ14">
-        <f>IF(U14&lt;&gt;"",(U$3/1000)*((U$3+1)-U14),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -2122,91 +2170,91 @@
       <c r="T15" s="9"/>
       <c r="U15" s="9"/>
       <c r="V15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="23"/>
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="W15" s="5" t="str">
-        <f>A15</f>
+        <f t="shared" si="2"/>
         <v>Roman Eazotov</v>
       </c>
       <c r="X15">
-        <f>IF(B15&lt;&gt;"",(B$3/1000)*((B$3+1)-B15),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y15">
-        <f>IF(C15&lt;&gt;"",(C$3/1000)*((C$3+1)-C15),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z15">
-        <f>IF(D15&lt;&gt;"",(D$3/1000)*((D$3+1)-D15),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA15">
-        <f>IF(E15&lt;&gt;"",(E$3/1000)*((E$3+1)-E15),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB15">
-        <f>IF(F15&lt;&gt;"",(F$3/1000)*((F$3+1)-F15),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC15">
-        <f>IF(G15&lt;&gt;"",(G$3/1000)*((G$3+1)-G15),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD15">
-        <f>IF(H15&lt;&gt;"",(H$3/1000)*((H$3+1)-H15),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE15">
-        <f>IF(I15&lt;&gt;"",(I$3/1000)*((I$3+1)-I15),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF15">
-        <f>IF(J15&lt;&gt;"",(J$3/1000)*((J$3+1)-J15),0)</f>
+        <f t="shared" si="11"/>
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="AG15">
-        <f>IF(K15&lt;&gt;"",(K$3/1000)*((K$3+1)-K15),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH15">
-        <f>IF(L15&lt;&gt;"",(L$3/1000)*((L$3+1)-L15),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI15">
-        <f>IF(M15&lt;&gt;"",(M$3/1000)*((M$3+1)-M15),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ15">
-        <f>IF(N15&lt;&gt;"",(N$3/1000)*((N$3+1)-N15),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK15">
-        <f>IF(O15&lt;&gt;"",(O$3/1000)*((O$3+1)-O15),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL15">
-        <f>IF(P15&lt;&gt;"",(P$3/1000)*((P$3+1)-P15),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM15">
-        <f>IF(Q15&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q15),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN15">
-        <f>IF(R15&lt;&gt;"",(R$3/1000)*((R$3+1)-R15),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO15">
-        <f>IF(S15&lt;&gt;"",(S$3/1000)*((S$3+1)-S15),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP15">
-        <f>IF(T15&lt;&gt;"",(T$3/1000)*((T$3+1)-T15),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ15">
-        <f>IF(U15&lt;&gt;"",(U$3/1000)*((U$3+1)-U15),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -2237,91 +2285,91 @@
       <c r="T16" s="9"/>
       <c r="U16" s="9"/>
       <c r="V16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="23"/>
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="W16" s="5" t="str">
-        <f>A16</f>
+        <f t="shared" si="2"/>
         <v>Sergey Bondarchuk</v>
       </c>
       <c r="X16">
-        <f>IF(B16&lt;&gt;"",(B$3/1000)*((B$3+1)-B16),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y16">
-        <f>IF(C16&lt;&gt;"",(C$3/1000)*((C$3+1)-C16),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z16">
-        <f>IF(D16&lt;&gt;"",(D$3/1000)*((D$3+1)-D16),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA16">
-        <f>IF(E16&lt;&gt;"",(E$3/1000)*((E$3+1)-E16),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB16">
-        <f>IF(F16&lt;&gt;"",(F$3/1000)*((F$3+1)-F16),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC16">
-        <f>IF(G16&lt;&gt;"",(G$3/1000)*((G$3+1)-G16),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD16">
-        <f>IF(H16&lt;&gt;"",(H$3/1000)*((H$3+1)-H16),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE16">
-        <f>IF(I16&lt;&gt;"",(I$3/1000)*((I$3+1)-I16),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF16">
-        <f>IF(J16&lt;&gt;"",(J$3/1000)*((J$3+1)-J16),0)</f>
+        <f t="shared" si="11"/>
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="AG16">
-        <f>IF(K16&lt;&gt;"",(K$3/1000)*((K$3+1)-K16),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH16">
-        <f>IF(L16&lt;&gt;"",(L$3/1000)*((L$3+1)-L16),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI16">
-        <f>IF(M16&lt;&gt;"",(M$3/1000)*((M$3+1)-M16),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ16">
-        <f>IF(N16&lt;&gt;"",(N$3/1000)*((N$3+1)-N16),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK16">
-        <f>IF(O16&lt;&gt;"",(O$3/1000)*((O$3+1)-O16),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL16">
-        <f>IF(P16&lt;&gt;"",(P$3/1000)*((P$3+1)-P16),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM16">
-        <f>IF(Q16&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q16),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN16">
-        <f>IF(R16&lt;&gt;"",(R$3/1000)*((R$3+1)-R16),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO16">
-        <f>IF(S16&lt;&gt;"",(S$3/1000)*((S$3+1)-S16),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP16">
-        <f>IF(T16&lt;&gt;"",(T$3/1000)*((T$3+1)-T16),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ16">
-        <f>IF(U16&lt;&gt;"",(U$3/1000)*((U$3+1)-U16),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -2360,7 +2408,9 @@
       <c r="L17" s="9">
         <v>4</v>
       </c>
-      <c r="M17" s="9"/>
+      <c r="M17" s="9">
+        <v>3</v>
+      </c>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
@@ -2370,91 +2420,91 @@
       <c r="T17" s="9"/>
       <c r="U17" s="9"/>
       <c r="V17">
-        <f t="shared" si="0"/>
-        <v>0.36200000000000004</v>
+        <f t="shared" si="23"/>
+        <v>0.41000000000000003</v>
       </c>
       <c r="W17" s="5" t="str">
-        <f>A17</f>
+        <f t="shared" si="2"/>
         <v>Alexandr Zakirov</v>
       </c>
       <c r="X17">
-        <f>IF(B17&lt;&gt;"",(B$3/1000)*((B$3+1)-B17),0)</f>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="Y17">
-        <f>IF(C17&lt;&gt;"",(C$3/1000)*((C$3+1)-C17),0)</f>
+        <f t="shared" si="4"/>
         <v>2.4E-2</v>
       </c>
       <c r="Z17">
-        <f>IF(D17&lt;&gt;"",(D$3/1000)*((D$3+1)-D17),0)</f>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="AA17">
-        <f>IF(E17&lt;&gt;"",(E$3/1000)*((E$3+1)-E17),0)</f>
+        <f t="shared" si="6"/>
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="AB17">
-        <f>IF(F17&lt;&gt;"",(F$3/1000)*((F$3+1)-F17),0)</f>
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
       <c r="AC17">
-        <f>IF(G17&lt;&gt;"",(G$3/1000)*((G$3+1)-G17),0)</f>
+        <f t="shared" si="8"/>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="AD17">
-        <f>IF(H17&lt;&gt;"",(H$3/1000)*((H$3+1)-H17),0)</f>
+        <f t="shared" si="9"/>
         <v>0.08</v>
       </c>
       <c r="AE17">
-        <f>IF(I17&lt;&gt;"",(I$3/1000)*((I$3+1)-I17),0)</f>
+        <f t="shared" si="10"/>
         <v>2.4E-2</v>
       </c>
       <c r="AF17">
-        <f>IF(J17&lt;&gt;"",(J$3/1000)*((J$3+1)-J17),0)</f>
+        <f t="shared" si="11"/>
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="AG17">
-        <f>IF(K17&lt;&gt;"",(K$3/1000)*((K$3+1)-K17),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH17">
-        <f>IF(L17&lt;&gt;"",(L$3/1000)*((L$3+1)-L17),0)</f>
+        <f t="shared" si="13"/>
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="AI17">
-        <f>IF(M17&lt;&gt;"",(M$3/1000)*((M$3+1)-M17),0)</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="AJ17">
-        <f>IF(N17&lt;&gt;"",(N$3/1000)*((N$3+1)-N17),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK17">
-        <f>IF(O17&lt;&gt;"",(O$3/1000)*((O$3+1)-O17),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL17">
-        <f>IF(P17&lt;&gt;"",(P$3/1000)*((P$3+1)-P17),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM17">
-        <f>IF(Q17&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q17),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN17">
-        <f>IF(R17&lt;&gt;"",(R$3/1000)*((R$3+1)-R17),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO17">
-        <f>IF(S17&lt;&gt;"",(S$3/1000)*((S$3+1)-S17),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP17">
-        <f>IF(T17&lt;&gt;"",(T$3/1000)*((T$3+1)-T17),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ17">
-        <f>IF(U17&lt;&gt;"",(U$3/1000)*((U$3+1)-U17),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -2491,91 +2541,91 @@
       <c r="T18" s="9"/>
       <c r="U18" s="9"/>
       <c r="V18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="23"/>
         <v>0.28199999999999997</v>
       </c>
       <c r="W18" s="5" t="str">
-        <f>A18</f>
+        <f t="shared" si="2"/>
         <v>Dmitry Ivanov</v>
       </c>
       <c r="X18">
-        <f>IF(B18&lt;&gt;"",(B$3/1000)*((B$3+1)-B18),0)</f>
+        <f t="shared" si="3"/>
         <v>0.09</v>
       </c>
       <c r="Y18">
-        <f>IF(C18&lt;&gt;"",(C$3/1000)*((C$3+1)-C18),0)</f>
+        <f t="shared" si="4"/>
         <v>0.03</v>
       </c>
       <c r="Z18">
-        <f>IF(D18&lt;&gt;"",(D$3/1000)*((D$3+1)-D18),0)</f>
+        <f t="shared" si="5"/>
         <v>0.09</v>
       </c>
       <c r="AA18">
-        <f>IF(E18&lt;&gt;"",(E$3/1000)*((E$3+1)-E18),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB18">
-        <f>IF(F18&lt;&gt;"",(F$3/1000)*((F$3+1)-F18),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC18">
-        <f>IF(G18&lt;&gt;"",(G$3/1000)*((G$3+1)-G18),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD18">
-        <f>IF(H18&lt;&gt;"",(H$3/1000)*((H$3+1)-H18),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE18">
-        <f>IF(I18&lt;&gt;"",(I$3/1000)*((I$3+1)-I18),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF18">
-        <f>IF(J18&lt;&gt;"",(J$3/1000)*((J$3+1)-J18),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG18">
-        <f>IF(K18&lt;&gt;"",(K$3/1000)*((K$3+1)-K18),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH18">
-        <f>IF(L18&lt;&gt;"",(L$3/1000)*((L$3+1)-L18),0)</f>
+        <f t="shared" si="13"/>
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="AI18">
-        <f>IF(M18&lt;&gt;"",(M$3/1000)*((M$3+1)-M18),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ18">
-        <f>IF(N18&lt;&gt;"",(N$3/1000)*((N$3+1)-N18),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK18">
-        <f>IF(O18&lt;&gt;"",(O$3/1000)*((O$3+1)-O18),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL18">
-        <f>IF(P18&lt;&gt;"",(P$3/1000)*((P$3+1)-P18),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM18">
-        <f>IF(Q18&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q18),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN18">
-        <f>IF(R18&lt;&gt;"",(R$3/1000)*((R$3+1)-R18),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO18">
-        <f>IF(S18&lt;&gt;"",(S$3/1000)*((S$3+1)-S18),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP18">
-        <f>IF(T18&lt;&gt;"",(T$3/1000)*((T$3+1)-T18),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ18">
-        <f>IF(U18&lt;&gt;"",(U$3/1000)*((U$3+1)-U18),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -2618,91 +2668,91 @@
       <c r="T19" s="9"/>
       <c r="U19" s="9"/>
       <c r="V19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="23"/>
         <v>0.32300000000000001</v>
       </c>
       <c r="W19" s="5" t="str">
-        <f>A19</f>
+        <f t="shared" si="2"/>
         <v>Axsan Kalimulin</v>
       </c>
       <c r="X19">
-        <f>IF(B19&lt;&gt;"",(B$3/1000)*((B$3+1)-B19),0)</f>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="Y19">
-        <f>IF(C19&lt;&gt;"",(C$3/1000)*((C$3+1)-C19),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z19">
-        <f>IF(D19&lt;&gt;"",(D$3/1000)*((D$3+1)-D19),0)</f>
+        <f t="shared" si="5"/>
         <v>0.08</v>
       </c>
       <c r="AA19">
-        <f>IF(E19&lt;&gt;"",(E$3/1000)*((E$3+1)-E19),0)</f>
+        <f t="shared" si="6"/>
         <v>6.3E-2</v>
       </c>
       <c r="AB19">
-        <f>IF(F19&lt;&gt;"",(F$3/1000)*((F$3+1)-F19),0)</f>
+        <f t="shared" si="7"/>
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="AC19">
-        <f>IF(G19&lt;&gt;"",(G$3/1000)*((G$3+1)-G19),0)</f>
+        <f t="shared" si="8"/>
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="AD19">
-        <f>IF(H19&lt;&gt;"",(H$3/1000)*((H$3+1)-H19),0)</f>
+        <f t="shared" si="9"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AE19">
-        <f>IF(I19&lt;&gt;"",(I$3/1000)*((I$3+1)-I19),0)</f>
+        <f t="shared" si="10"/>
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="AF19">
-        <f>IF(J19&lt;&gt;"",(J$3/1000)*((J$3+1)-J19),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG19">
-        <f>IF(K19&lt;&gt;"",(K$3/1000)*((K$3+1)-K19),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH19">
-        <f>IF(L19&lt;&gt;"",(L$3/1000)*((L$3+1)-L19),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI19">
-        <f>IF(M19&lt;&gt;"",(M$3/1000)*((M$3+1)-M19),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ19">
-        <f>IF(N19&lt;&gt;"",(N$3/1000)*((N$3+1)-N19),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK19">
-        <f>IF(O19&lt;&gt;"",(O$3/1000)*((O$3+1)-O19),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL19">
-        <f>IF(P19&lt;&gt;"",(P$3/1000)*((P$3+1)-P19),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM19">
-        <f>IF(Q19&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q19),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN19">
-        <f>IF(R19&lt;&gt;"",(R$3/1000)*((R$3+1)-R19),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO19">
-        <f>IF(S19&lt;&gt;"",(S$3/1000)*((S$3+1)-S19),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP19">
-        <f>IF(T19&lt;&gt;"",(T$3/1000)*((T$3+1)-T19),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ19">
-        <f>IF(U19&lt;&gt;"",(U$3/1000)*((U$3+1)-U19),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -2735,91 +2785,91 @@
       <c r="T20" s="9"/>
       <c r="U20" s="9"/>
       <c r="V20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="23"/>
         <v>6.2E-2</v>
       </c>
       <c r="W20" s="5" t="str">
-        <f>A20</f>
+        <f t="shared" si="2"/>
         <v>Nikita Kashin</v>
       </c>
       <c r="X20">
-        <f>IF(B20&lt;&gt;"",(B$3/1000)*((B$3+1)-B20),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y20">
-        <f>IF(C20&lt;&gt;"",(C$3/1000)*((C$3+1)-C20),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z20">
-        <f>IF(D20&lt;&gt;"",(D$3/1000)*((D$3+1)-D20),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA20">
-        <f>IF(E20&lt;&gt;"",(E$3/1000)*((E$3+1)-E20),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB20">
-        <f>IF(F20&lt;&gt;"",(F$3/1000)*((F$3+1)-F20),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC20">
-        <f>IF(G20&lt;&gt;"",(G$3/1000)*((G$3+1)-G20),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD20">
-        <f>IF(H20&lt;&gt;"",(H$3/1000)*((H$3+1)-H20),0)</f>
+        <f t="shared" si="9"/>
         <v>0.03</v>
       </c>
       <c r="AE20">
-        <f>IF(I20&lt;&gt;"",(I$3/1000)*((I$3+1)-I20),0)</f>
+        <f t="shared" si="10"/>
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="AF20">
-        <f>IF(J20&lt;&gt;"",(J$3/1000)*((J$3+1)-J20),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG20">
-        <f>IF(K20&lt;&gt;"",(K$3/1000)*((K$3+1)-K20),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH20">
-        <f>IF(L20&lt;&gt;"",(L$3/1000)*((L$3+1)-L20),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI20">
-        <f>IF(M20&lt;&gt;"",(M$3/1000)*((M$3+1)-M20),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ20">
-        <f>IF(N20&lt;&gt;"",(N$3/1000)*((N$3+1)-N20),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK20">
-        <f>IF(O20&lt;&gt;"",(O$3/1000)*((O$3+1)-O20),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL20">
-        <f>IF(P20&lt;&gt;"",(P$3/1000)*((P$3+1)-P20),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM20">
-        <f>IF(Q20&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q20),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN20">
-        <f>IF(R20&lt;&gt;"",(R$3/1000)*((R$3+1)-R20),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO20">
-        <f>IF(S20&lt;&gt;"",(S$3/1000)*((S$3+1)-S20),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP20">
-        <f>IF(T20&lt;&gt;"",(T$3/1000)*((T$3+1)-T20),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ20">
-        <f>IF(U20&lt;&gt;"",(U$3/1000)*((U$3+1)-U20),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -2852,91 +2902,91 @@
       <c r="T21" s="9"/>
       <c r="U21" s="9"/>
       <c r="V21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="23"/>
         <v>0.05</v>
       </c>
       <c r="W21" s="5" t="str">
-        <f>A21</f>
+        <f t="shared" si="2"/>
         <v>Andrey Korneev</v>
       </c>
       <c r="X21">
-        <f>IF(B21&lt;&gt;"",(B$3/1000)*((B$3+1)-B21),0)</f>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
       <c r="Y21">
-        <f>IF(C21&lt;&gt;"",(C$3/1000)*((C$3+1)-C21),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z21">
-        <f>IF(D21&lt;&gt;"",(D$3/1000)*((D$3+1)-D21),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA21">
-        <f>IF(E21&lt;&gt;"",(E$3/1000)*((E$3+1)-E21),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB21">
-        <f>IF(F21&lt;&gt;"",(F$3/1000)*((F$3+1)-F21),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC21">
-        <f>IF(G21&lt;&gt;"",(G$3/1000)*((G$3+1)-G21),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD21">
-        <f>IF(H21&lt;&gt;"",(H$3/1000)*((H$3+1)-H21),0)</f>
+        <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
       <c r="AE21">
-        <f>IF(I21&lt;&gt;"",(I$3/1000)*((I$3+1)-I21),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF21">
-        <f>IF(J21&lt;&gt;"",(J$3/1000)*((J$3+1)-J21),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG21">
-        <f>IF(K21&lt;&gt;"",(K$3/1000)*((K$3+1)-K21),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH21">
-        <f>IF(L21&lt;&gt;"",(L$3/1000)*((L$3+1)-L21),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI21">
-        <f>IF(M21&lt;&gt;"",(M$3/1000)*((M$3+1)-M21),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ21">
-        <f>IF(N21&lt;&gt;"",(N$3/1000)*((N$3+1)-N21),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK21">
-        <f>IF(O21&lt;&gt;"",(O$3/1000)*((O$3+1)-O21),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL21">
-        <f>IF(P21&lt;&gt;"",(P$3/1000)*((P$3+1)-P21),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM21">
-        <f>IF(Q21&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q21),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN21">
-        <f>IF(R21&lt;&gt;"",(R$3/1000)*((R$3+1)-R21),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO21">
-        <f>IF(S21&lt;&gt;"",(S$3/1000)*((S$3+1)-S21),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP21">
-        <f>IF(T21&lt;&gt;"",(T$3/1000)*((T$3+1)-T21),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ21">
-        <f>IF(U21&lt;&gt;"",(U$3/1000)*((U$3+1)-U21),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -2973,91 +3023,91 @@
       <c r="T22" s="9"/>
       <c r="U22" s="9"/>
       <c r="V22">
-        <f t="shared" ref="V22" si="1">SUM(X22:AN22)</f>
+        <f t="shared" ref="V22" si="24">SUM(X22:AN22)</f>
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="W22" s="5" t="str">
-        <f>A22</f>
+        <f t="shared" si="2"/>
         <v>Alexey Makeev</v>
       </c>
       <c r="X22">
-        <f>IF(B22&lt;&gt;"",(B$3/1000)*((B$3+1)-B22),0)</f>
+        <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
       <c r="Y22">
-        <f>IF(C22&lt;&gt;"",(C$3/1000)*((C$3+1)-C22),0)</f>
+        <f t="shared" si="4"/>
         <v>1.2E-2</v>
       </c>
       <c r="Z22">
-        <f>IF(D22&lt;&gt;"",(D$3/1000)*((D$3+1)-D22),0)</f>
+        <f t="shared" si="5"/>
         <v>0.05</v>
       </c>
       <c r="AA22">
-        <f>IF(E22&lt;&gt;"",(E$3/1000)*((E$3+1)-E22),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB22">
-        <f>IF(F22&lt;&gt;"",(F$3/1000)*((F$3+1)-F22),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC22">
-        <f>IF(G22&lt;&gt;"",(G$3/1000)*((G$3+1)-G22),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD22">
-        <f>IF(H22&lt;&gt;"",(H$3/1000)*((H$3+1)-H22),0)</f>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="AE22">
-        <f>IF(I22&lt;&gt;"",(I$3/1000)*((I$3+1)-I22),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF22">
-        <f>IF(J22&lt;&gt;"",(J$3/1000)*((J$3+1)-J22),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG22">
-        <f>IF(K22&lt;&gt;"",(K$3/1000)*((K$3+1)-K22),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH22">
-        <f>IF(L22&lt;&gt;"",(L$3/1000)*((L$3+1)-L22),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI22">
-        <f>IF(M22&lt;&gt;"",(M$3/1000)*((M$3+1)-M22),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ22">
-        <f>IF(N22&lt;&gt;"",(N$3/1000)*((N$3+1)-N22),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK22">
-        <f>IF(O22&lt;&gt;"",(O$3/1000)*((O$3+1)-O22),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL22">
-        <f>IF(P22&lt;&gt;"",(P$3/1000)*((P$3+1)-P22),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM22">
-        <f>IF(Q22&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q22),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN22">
-        <f>IF(R22&lt;&gt;"",(R$3/1000)*((R$3+1)-R22),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO22">
-        <f>IF(S22&lt;&gt;"",(S$3/1000)*((S$3+1)-S22),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP22">
-        <f>IF(T22&lt;&gt;"",(T$3/1000)*((T$3+1)-T22),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ22">
-        <f>IF(U22&lt;&gt;"",(U$3/1000)*((U$3+1)-U22),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -3088,91 +3138,91 @@
       <c r="T23" s="9"/>
       <c r="U23" s="9"/>
       <c r="V23">
-        <f t="shared" ref="V23:V32" si="2">SUM(X23:AN23)</f>
+        <f t="shared" ref="V23:V32" si="25">SUM(X23:AN23)</f>
         <v>0.08</v>
       </c>
       <c r="W23" s="5" t="str">
-        <f>A23</f>
+        <f t="shared" si="2"/>
         <v>Robert Mardanov</v>
       </c>
       <c r="X23">
-        <f>IF(B23&lt;&gt;"",(B$3/1000)*((B$3+1)-B23),0)</f>
+        <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
       <c r="Y23">
-        <f>IF(C23&lt;&gt;"",(C$3/1000)*((C$3+1)-C23),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z23">
-        <f>IF(D23&lt;&gt;"",(D$3/1000)*((D$3+1)-D23),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA23">
-        <f>IF(E23&lt;&gt;"",(E$3/1000)*((E$3+1)-E23),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB23">
-        <f>IF(F23&lt;&gt;"",(F$3/1000)*((F$3+1)-F23),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC23">
-        <f>IF(G23&lt;&gt;"",(G$3/1000)*((G$3+1)-G23),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD23">
-        <f>IF(H23&lt;&gt;"",(H$3/1000)*((H$3+1)-H23),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE23">
-        <f>IF(I23&lt;&gt;"",(I$3/1000)*((I$3+1)-I23),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF23">
-        <f>IF(J23&lt;&gt;"",(J$3/1000)*((J$3+1)-J23),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG23">
-        <f>IF(K23&lt;&gt;"",(K$3/1000)*((K$3+1)-K23),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH23">
-        <f>IF(L23&lt;&gt;"",(L$3/1000)*((L$3+1)-L23),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI23">
-        <f>IF(M23&lt;&gt;"",(M$3/1000)*((M$3+1)-M23),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ23">
-        <f>IF(N23&lt;&gt;"",(N$3/1000)*((N$3+1)-N23),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK23">
-        <f>IF(O23&lt;&gt;"",(O$3/1000)*((O$3+1)-O23),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL23">
-        <f>IF(P23&lt;&gt;"",(P$3/1000)*((P$3+1)-P23),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM23">
-        <f>IF(Q23&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q23),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN23">
-        <f>IF(R23&lt;&gt;"",(R$3/1000)*((R$3+1)-R23),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO23">
-        <f>IF(S23&lt;&gt;"",(S$3/1000)*((S$3+1)-S23),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP23">
-        <f>IF(T23&lt;&gt;"",(T$3/1000)*((T$3+1)-T23),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ23">
-        <f>IF(U23&lt;&gt;"",(U$3/1000)*((U$3+1)-U23),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -3205,91 +3255,91 @@
       <c r="T24" s="9"/>
       <c r="U24" s="9"/>
       <c r="V24">
+        <f t="shared" si="25"/>
+        <v>0.14200000000000002</v>
+      </c>
+      <c r="W24" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.14200000000000002</v>
-      </c>
-      <c r="W24" s="5" t="str">
-        <f>A24</f>
         <v>Petr Myakushin</v>
       </c>
       <c r="X24">
-        <f>IF(B24&lt;&gt;"",(B$3/1000)*((B$3+1)-B24),0)</f>
+        <f t="shared" si="3"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="Y24">
-        <f>IF(C24&lt;&gt;"",(C$3/1000)*((C$3+1)-C24),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z24">
-        <f>IF(D24&lt;&gt;"",(D$3/1000)*((D$3+1)-D24),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA24">
-        <f>IF(E24&lt;&gt;"",(E$3/1000)*((E$3+1)-E24),0)</f>
+        <f t="shared" si="6"/>
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="AB24">
-        <f>IF(F24&lt;&gt;"",(F$3/1000)*((F$3+1)-F24),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC24">
-        <f>IF(G24&lt;&gt;"",(G$3/1000)*((G$3+1)-G24),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD24">
-        <f>IF(H24&lt;&gt;"",(H$3/1000)*((H$3+1)-H24),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE24">
-        <f>IF(I24&lt;&gt;"",(I$3/1000)*((I$3+1)-I24),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF24">
-        <f>IF(J24&lt;&gt;"",(J$3/1000)*((J$3+1)-J24),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG24">
-        <f>IF(K24&lt;&gt;"",(K$3/1000)*((K$3+1)-K24),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH24">
-        <f>IF(L24&lt;&gt;"",(L$3/1000)*((L$3+1)-L24),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI24">
-        <f>IF(M24&lt;&gt;"",(M$3/1000)*((M$3+1)-M24),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ24">
-        <f>IF(N24&lt;&gt;"",(N$3/1000)*((N$3+1)-N24),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK24">
-        <f>IF(O24&lt;&gt;"",(O$3/1000)*((O$3+1)-O24),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL24">
-        <f>IF(P24&lt;&gt;"",(P$3/1000)*((P$3+1)-P24),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM24">
-        <f>IF(Q24&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q24),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN24">
-        <f>IF(R24&lt;&gt;"",(R$3/1000)*((R$3+1)-R24),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO24">
-        <f>IF(S24&lt;&gt;"",(S$3/1000)*((S$3+1)-S24),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP24">
-        <f>IF(T24&lt;&gt;"",(T$3/1000)*((T$3+1)-T24),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ24">
-        <f>IF(U24&lt;&gt;"",(U$3/1000)*((U$3+1)-U24),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -3322,91 +3372,91 @@
       <c r="T25" s="9"/>
       <c r="U25" s="9"/>
       <c r="V25">
+        <f t="shared" si="25"/>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="W25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="W25" s="5" t="str">
-        <f>A25</f>
         <v>Artem Gusev</v>
       </c>
       <c r="X25">
-        <f>IF(B25&lt;&gt;"",(B$3/1000)*((B$3+1)-B25),0)</f>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
       <c r="Y25">
-        <f>IF(C25&lt;&gt;"",(C$3/1000)*((C$3+1)-C25),0)</f>
+        <f t="shared" si="4"/>
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="Z25">
-        <f>IF(D25&lt;&gt;"",(D$3/1000)*((D$3+1)-D25),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA25">
-        <f>IF(E25&lt;&gt;"",(E$3/1000)*((E$3+1)-E25),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB25">
-        <f>IF(F25&lt;&gt;"",(F$3/1000)*((F$3+1)-F25),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC25">
-        <f>IF(G25&lt;&gt;"",(G$3/1000)*((G$3+1)-G25),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD25">
-        <f>IF(H25&lt;&gt;"",(H$3/1000)*((H$3+1)-H25),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE25">
-        <f>IF(I25&lt;&gt;"",(I$3/1000)*((I$3+1)-I25),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF25">
-        <f>IF(J25&lt;&gt;"",(J$3/1000)*((J$3+1)-J25),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG25">
-        <f>IF(K25&lt;&gt;"",(K$3/1000)*((K$3+1)-K25),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH25">
-        <f>IF(L25&lt;&gt;"",(L$3/1000)*((L$3+1)-L25),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI25">
-        <f>IF(M25&lt;&gt;"",(M$3/1000)*((M$3+1)-M25),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ25">
-        <f>IF(N25&lt;&gt;"",(N$3/1000)*((N$3+1)-N25),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK25">
-        <f>IF(O25&lt;&gt;"",(O$3/1000)*((O$3+1)-O25),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL25">
-        <f>IF(P25&lt;&gt;"",(P$3/1000)*((P$3+1)-P25),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM25">
-        <f>IF(Q25&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q25),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN25">
-        <f>IF(R25&lt;&gt;"",(R$3/1000)*((R$3+1)-R25),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO25">
-        <f>IF(S25&lt;&gt;"",(S$3/1000)*((S$3+1)-S25),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP25">
-        <f>IF(T25&lt;&gt;"",(T$3/1000)*((T$3+1)-T25),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ25">
-        <f>IF(U25&lt;&gt;"",(U$3/1000)*((U$3+1)-U25),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -3439,91 +3489,91 @@
       <c r="T26" s="9"/>
       <c r="U26" s="9"/>
       <c r="V26">
+        <f t="shared" si="25"/>
+        <v>3.9E-2</v>
+      </c>
+      <c r="W26" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>3.9E-2</v>
-      </c>
-      <c r="W26" s="5" t="str">
-        <f>A26</f>
         <v>Yury Sbitnev</v>
       </c>
       <c r="X26">
-        <f>IF(B26&lt;&gt;"",(B$3/1000)*((B$3+1)-B26),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y26">
-        <f>IF(C26&lt;&gt;"",(C$3/1000)*((C$3+1)-C26),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z26">
-        <f>IF(D26&lt;&gt;"",(D$3/1000)*((D$3+1)-D26),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA26">
-        <f>IF(E26&lt;&gt;"",(E$3/1000)*((E$3+1)-E26),0)</f>
+        <f t="shared" si="6"/>
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="AB26">
-        <f>IF(F26&lt;&gt;"",(F$3/1000)*((F$3+1)-F26),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC26">
-        <f>IF(G26&lt;&gt;"",(G$3/1000)*((G$3+1)-G26),0)</f>
+        <f t="shared" si="8"/>
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="AD26">
-        <f>IF(H26&lt;&gt;"",(H$3/1000)*((H$3+1)-H26),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE26">
-        <f>IF(I26&lt;&gt;"",(I$3/1000)*((I$3+1)-I26),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF26">
-        <f>IF(J26&lt;&gt;"",(J$3/1000)*((J$3+1)-J26),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG26">
-        <f>IF(K26&lt;&gt;"",(K$3/1000)*((K$3+1)-K26),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH26">
-        <f>IF(L26&lt;&gt;"",(L$3/1000)*((L$3+1)-L26),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI26">
-        <f>IF(M26&lt;&gt;"",(M$3/1000)*((M$3+1)-M26),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ26">
-        <f>IF(N26&lt;&gt;"",(N$3/1000)*((N$3+1)-N26),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK26">
-        <f>IF(O26&lt;&gt;"",(O$3/1000)*((O$3+1)-O26),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL26">
-        <f>IF(P26&lt;&gt;"",(P$3/1000)*((P$3+1)-P26),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM26">
-        <f>IF(Q26&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q26),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN26">
-        <f>IF(R26&lt;&gt;"",(R$3/1000)*((R$3+1)-R26),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO26">
-        <f>IF(S26&lt;&gt;"",(S$3/1000)*((S$3+1)-S26),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP26">
-        <f>IF(T26&lt;&gt;"",(T$3/1000)*((T$3+1)-T26),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ26">
-        <f>IF(U26&lt;&gt;"",(U$3/1000)*((U$3+1)-U26),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -3554,91 +3604,91 @@
       <c r="T27" s="9"/>
       <c r="U27" s="9"/>
       <c r="V27">
+        <f t="shared" si="25"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W27" s="5" t="str">
         <f t="shared" si="2"/>
+        <v>Sergey Mazurin</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="W27" s="5" t="str">
-        <f>A27</f>
-        <v>Sergey Mazurin</v>
-      </c>
-      <c r="X27">
-        <f>IF(B27&lt;&gt;"",(B$3/1000)*((B$3+1)-B27),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y27">
-        <f>IF(C27&lt;&gt;"",(C$3/1000)*((C$3+1)-C27),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z27">
-        <f>IF(D27&lt;&gt;"",(D$3/1000)*((D$3+1)-D27),0)</f>
-        <v>7.0000000000000007E-2</v>
-      </c>
       <c r="AA27">
-        <f>IF(E27&lt;&gt;"",(E$3/1000)*((E$3+1)-E27),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB27">
-        <f>IF(F27&lt;&gt;"",(F$3/1000)*((F$3+1)-F27),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC27">
-        <f>IF(G27&lt;&gt;"",(G$3/1000)*((G$3+1)-G27),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD27">
-        <f>IF(H27&lt;&gt;"",(H$3/1000)*((H$3+1)-H27),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE27">
-        <f>IF(I27&lt;&gt;"",(I$3/1000)*((I$3+1)-I27),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF27">
-        <f>IF(J27&lt;&gt;"",(J$3/1000)*((J$3+1)-J27),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG27">
-        <f>IF(K27&lt;&gt;"",(K$3/1000)*((K$3+1)-K27),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH27">
-        <f>IF(L27&lt;&gt;"",(L$3/1000)*((L$3+1)-L27),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI27">
-        <f>IF(M27&lt;&gt;"",(M$3/1000)*((M$3+1)-M27),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ27">
-        <f>IF(N27&lt;&gt;"",(N$3/1000)*((N$3+1)-N27),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK27">
-        <f>IF(O27&lt;&gt;"",(O$3/1000)*((O$3+1)-O27),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL27">
-        <f>IF(P27&lt;&gt;"",(P$3/1000)*((P$3+1)-P27),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM27">
-        <f>IF(Q27&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q27),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN27">
-        <f>IF(R27&lt;&gt;"",(R$3/1000)*((R$3+1)-R27),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO27">
-        <f>IF(S27&lt;&gt;"",(S$3/1000)*((S$3+1)-S27),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP27">
-        <f>IF(T27&lt;&gt;"",(T$3/1000)*((T$3+1)-T27),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ27">
-        <f>IF(U27&lt;&gt;"",(U$3/1000)*((U$3+1)-U27),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -3669,91 +3719,91 @@
       <c r="T28" s="9"/>
       <c r="U28" s="9"/>
       <c r="V28">
+        <f t="shared" si="25"/>
+        <v>0.01</v>
+      </c>
+      <c r="W28" s="5" t="str">
         <f t="shared" si="2"/>
+        <v>Sergey Protiv</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="5"/>
         <v>0.01</v>
       </c>
-      <c r="W28" s="5" t="str">
-        <f>A28</f>
-        <v>Sergey Protiv</v>
-      </c>
-      <c r="X28">
-        <f>IF(B28&lt;&gt;"",(B$3/1000)*((B$3+1)-B28),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y28">
-        <f>IF(C28&lt;&gt;"",(C$3/1000)*((C$3+1)-C28),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z28">
-        <f>IF(D28&lt;&gt;"",(D$3/1000)*((D$3+1)-D28),0)</f>
-        <v>0.01</v>
-      </c>
       <c r="AA28">
-        <f>IF(E28&lt;&gt;"",(E$3/1000)*((E$3+1)-E28),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB28">
-        <f>IF(F28&lt;&gt;"",(F$3/1000)*((F$3+1)-F28),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC28">
-        <f>IF(G28&lt;&gt;"",(G$3/1000)*((G$3+1)-G28),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD28">
-        <f>IF(H28&lt;&gt;"",(H$3/1000)*((H$3+1)-H28),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE28">
-        <f>IF(I28&lt;&gt;"",(I$3/1000)*((I$3+1)-I28),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF28">
-        <f>IF(J28&lt;&gt;"",(J$3/1000)*((J$3+1)-J28),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG28">
-        <f>IF(K28&lt;&gt;"",(K$3/1000)*((K$3+1)-K28),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH28">
-        <f>IF(L28&lt;&gt;"",(L$3/1000)*((L$3+1)-L28),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI28">
-        <f>IF(M28&lt;&gt;"",(M$3/1000)*((M$3+1)-M28),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ28">
-        <f>IF(N28&lt;&gt;"",(N$3/1000)*((N$3+1)-N28),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK28">
-        <f>IF(O28&lt;&gt;"",(O$3/1000)*((O$3+1)-O28),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL28">
-        <f>IF(P28&lt;&gt;"",(P$3/1000)*((P$3+1)-P28),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM28">
-        <f>IF(Q28&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q28),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN28">
-        <f>IF(R28&lt;&gt;"",(R$3/1000)*((R$3+1)-R28),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO28">
-        <f>IF(S28&lt;&gt;"",(S$3/1000)*((S$3+1)-S28),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP28">
-        <f>IF(T28&lt;&gt;"",(T$3/1000)*((T$3+1)-T28),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ28">
-        <f>IF(U28&lt;&gt;"",(U$3/1000)*((U$3+1)-U28),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -3784,96 +3834,98 @@
       <c r="T29" s="9"/>
       <c r="U29" s="9"/>
       <c r="V29">
+        <f t="shared" si="25"/>
+        <v>0.03</v>
+      </c>
+      <c r="W29" s="5" t="str">
         <f t="shared" si="2"/>
+        <v>Nikolay Kondratev</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="5"/>
         <v>0.03</v>
       </c>
-      <c r="W29" s="5" t="str">
-        <f>A29</f>
-        <v>Nikolay Kondratev</v>
-      </c>
-      <c r="X29">
-        <f>IF(B29&lt;&gt;"",(B$3/1000)*((B$3+1)-B29),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y29">
-        <f>IF(C29&lt;&gt;"",(C$3/1000)*((C$3+1)-C29),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z29">
-        <f>IF(D29&lt;&gt;"",(D$3/1000)*((D$3+1)-D29),0)</f>
-        <v>0.03</v>
-      </c>
       <c r="AA29">
-        <f>IF(E29&lt;&gt;"",(E$3/1000)*((E$3+1)-E29),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB29">
-        <f>IF(F29&lt;&gt;"",(F$3/1000)*((F$3+1)-F29),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC29">
-        <f>IF(G29&lt;&gt;"",(G$3/1000)*((G$3+1)-G29),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD29">
-        <f>IF(H29&lt;&gt;"",(H$3/1000)*((H$3+1)-H29),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE29">
-        <f>IF(I29&lt;&gt;"",(I$3/1000)*((I$3+1)-I29),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF29">
-        <f>IF(J29&lt;&gt;"",(J$3/1000)*((J$3+1)-J29),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG29">
-        <f>IF(K29&lt;&gt;"",(K$3/1000)*((K$3+1)-K29),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH29">
-        <f>IF(L29&lt;&gt;"",(L$3/1000)*((L$3+1)-L29),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI29">
-        <f>IF(M29&lt;&gt;"",(M$3/1000)*((M$3+1)-M29),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ29">
-        <f>IF(N29&lt;&gt;"",(N$3/1000)*((N$3+1)-N29),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK29">
-        <f>IF(O29&lt;&gt;"",(O$3/1000)*((O$3+1)-O29),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL29">
-        <f>IF(P29&lt;&gt;"",(P$3/1000)*((P$3+1)-P29),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM29">
-        <f>IF(Q29&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q29),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN29">
-        <f>IF(R29&lt;&gt;"",(R$3/1000)*((R$3+1)-R29),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO29">
-        <f>IF(S29&lt;&gt;"",(S$3/1000)*((S$3+1)-S29),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP29">
-        <f>IF(T29&lt;&gt;"",(T$3/1000)*((T$3+1)-T29),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ29">
-        <f>IF(U29&lt;&gt;"",(U$3/1000)*((U$3+1)-U29),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+      <c r="A30" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -3885,7 +3937,9 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
+      <c r="M30" s="9">
+        <v>7</v>
+      </c>
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
@@ -3895,91 +3949,91 @@
       <c r="T30" s="9"/>
       <c r="U30" s="9"/>
       <c r="V30">
+        <f t="shared" si="25"/>
+        <v>1.6E-2</v>
+      </c>
+      <c r="W30" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="W30" s="5">
-        <f>A30</f>
-        <v>0</v>
+        <v>Ilya Ivashchenko</v>
       </c>
       <c r="X30">
-        <f>IF(B30&lt;&gt;"",(B$3/1000)*((B$3+1)-B30),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y30">
-        <f>IF(C30&lt;&gt;"",(C$3/1000)*((C$3+1)-C30),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z30">
-        <f>IF(D30&lt;&gt;"",(D$3/1000)*((D$3+1)-D30),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA30">
-        <f>IF(E30&lt;&gt;"",(E$3/1000)*((E$3+1)-E30),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB30">
-        <f>IF(F30&lt;&gt;"",(F$3/1000)*((F$3+1)-F30),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC30">
-        <f>IF(G30&lt;&gt;"",(G$3/1000)*((G$3+1)-G30),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD30">
-        <f>IF(H30&lt;&gt;"",(H$3/1000)*((H$3+1)-H30),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE30">
-        <f>IF(I30&lt;&gt;"",(I$3/1000)*((I$3+1)-I30),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF30">
-        <f>IF(J30&lt;&gt;"",(J$3/1000)*((J$3+1)-J30),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG30">
-        <f>IF(K30&lt;&gt;"",(K$3/1000)*((K$3+1)-K30),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH30">
-        <f>IF(L30&lt;&gt;"",(L$3/1000)*((L$3+1)-L30),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI30">
-        <f>IF(M30&lt;&gt;"",(M$3/1000)*((M$3+1)-M30),0)</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>1.6E-2</v>
       </c>
       <c r="AJ30">
-        <f>IF(N30&lt;&gt;"",(N$3/1000)*((N$3+1)-N30),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK30">
-        <f>IF(O30&lt;&gt;"",(O$3/1000)*((O$3+1)-O30),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL30">
-        <f>IF(P30&lt;&gt;"",(P$3/1000)*((P$3+1)-P30),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM30">
-        <f>IF(Q30&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q30),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN30">
-        <f>IF(R30&lt;&gt;"",(R$3/1000)*((R$3+1)-R30),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO30">
-        <f>IF(S30&lt;&gt;"",(S$3/1000)*((S$3+1)-S30),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP30">
-        <f>IF(T30&lt;&gt;"",(T$3/1000)*((T$3+1)-T30),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ30">
-        <f>IF(U30&lt;&gt;"",(U$3/1000)*((U$3+1)-U30),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -4006,91 +4060,91 @@
       <c r="T31" s="9"/>
       <c r="U31" s="9"/>
       <c r="V31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W31" s="5">
-        <f t="shared" ref="W31:W32" si="3">A31</f>
+        <f t="shared" ref="W31:W32" si="26">A31</f>
         <v>0</v>
       </c>
       <c r="X31">
-        <f>IF(B31&lt;&gt;"",(B$3/1000)*((B$3+1)-B31),0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y31">
-        <f>IF(C31&lt;&gt;"",(C$3/1000)*((C$3+1)-C31),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z31">
-        <f>IF(D31&lt;&gt;"",(D$3/1000)*((D$3+1)-D31),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA31">
-        <f>IF(E31&lt;&gt;"",(E$3/1000)*((E$3+1)-E31),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB31">
-        <f>IF(F31&lt;&gt;"",(F$3/1000)*((F$3+1)-F31),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC31">
-        <f>IF(G31&lt;&gt;"",(G$3/1000)*((G$3+1)-G31),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD31">
-        <f>IF(H31&lt;&gt;"",(H$3/1000)*((H$3+1)-H31),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE31">
-        <f>IF(I31&lt;&gt;"",(I$3/1000)*((I$3+1)-I31),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF31">
-        <f>IF(J31&lt;&gt;"",(J$3/1000)*((J$3+1)-J31),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG31">
-        <f>IF(K31&lt;&gt;"",(K$3/1000)*((K$3+1)-K31),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH31">
-        <f>IF(L31&lt;&gt;"",(L$3/1000)*((L$3+1)-L31),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI31">
-        <f>IF(M31&lt;&gt;"",(M$3/1000)*((M$3+1)-M31),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ31">
-        <f>IF(N31&lt;&gt;"",(N$3/1000)*((N$3+1)-N31),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK31">
-        <f>IF(O31&lt;&gt;"",(O$3/1000)*((O$3+1)-O31),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL31">
-        <f>IF(P31&lt;&gt;"",(P$3/1000)*((P$3+1)-P31),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM31">
-        <f>IF(Q31&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q31),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN31">
-        <f>IF(R31&lt;&gt;"",(R$3/1000)*((R$3+1)-R31),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO31">
-        <f>IF(S31&lt;&gt;"",(S$3/1000)*((S$3+1)-S31),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP31">
-        <f>IF(T31&lt;&gt;"",(T$3/1000)*((T$3+1)-T31),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ31">
-        <f>IF(U31&lt;&gt;"",(U$3/1000)*((U$3+1)-U31),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -4117,91 +4171,91 @@
       <c r="T32" s="9"/>
       <c r="U32" s="9"/>
       <c r="V32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W32" s="5">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="X32">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X32">
-        <f>IF(B32&lt;&gt;"",(B$3/1000)*((B$3+1)-B32),0)</f>
-        <v>0</v>
-      </c>
       <c r="Y32">
-        <f>IF(C32&lt;&gt;"",(C$3/1000)*((C$3+1)-C32),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z32">
-        <f>IF(D32&lt;&gt;"",(D$3/1000)*((D$3+1)-D32),0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA32">
-        <f>IF(E32&lt;&gt;"",(E$3/1000)*((E$3+1)-E32),0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB32">
-        <f>IF(F32&lt;&gt;"",(F$3/1000)*((F$3+1)-F32),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC32">
-        <f>IF(G32&lt;&gt;"",(G$3/1000)*((G$3+1)-G32),0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD32">
-        <f>IF(H32&lt;&gt;"",(H$3/1000)*((H$3+1)-H32),0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AE32">
-        <f>IF(I32&lt;&gt;"",(I$3/1000)*((I$3+1)-I32),0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AF32">
-        <f>IF(J32&lt;&gt;"",(J$3/1000)*((J$3+1)-J32),0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG32">
-        <f>IF(K32&lt;&gt;"",(K$3/1000)*((K$3+1)-K32),0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH32">
-        <f>IF(L32&lt;&gt;"",(L$3/1000)*((L$3+1)-L32),0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AI32">
-        <f>IF(M32&lt;&gt;"",(M$3/1000)*((M$3+1)-M32),0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AJ32">
-        <f>IF(N32&lt;&gt;"",(N$3/1000)*((N$3+1)-N32),0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AK32">
-        <f>IF(O32&lt;&gt;"",(O$3/1000)*((O$3+1)-O32),0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AL32">
-        <f>IF(P32&lt;&gt;"",(P$3/1000)*((P$3+1)-P32),0)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AM32">
-        <f>IF(Q32&lt;&gt;"",(Q$3/1000)*((Q$3+1)-Q32),0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AN32">
-        <f>IF(R32&lt;&gt;"",(R$3/1000)*((R$3+1)-R32),0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AO32">
-        <f>IF(S32&lt;&gt;"",(S$3/1000)*((S$3+1)-S32),0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AP32">
-        <f>IF(T32&lt;&gt;"",(T$3/1000)*((T$3+1)-T32),0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AQ32">
-        <f>IF(U32&lt;&gt;"",(U$3/1000)*((U$3+1)-U32),0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -4213,17 +4267,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4231,285 +4285,296 @@
         <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="14">
+        <v>0.85399999999999987</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>2</v>
-      </c>
-      <c r="C2">
-        <v>0.78999999999999992</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="14">
+        <v>0.41000000000000003</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>16</v>
-      </c>
-      <c r="C3">
-        <v>0.36200000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="14">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>7</v>
-      </c>
-      <c r="C4">
-        <v>0.35599999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>0.32300000000000001</v>
+      <c r="B5" s="14">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>0.32099999999999995</v>
+      <c r="B6" s="14">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>0.30399999999999999</v>
+      <c r="B7" s="14">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="14">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="C8">
-        <v>0.28199999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="14">
+        <v>0.21799999999999997</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>4</v>
-      </c>
-      <c r="C9">
-        <v>0.16199999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10">
-        <v>0.14200000000000002</v>
+      <c r="B10" s="14">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>0.126</v>
+      <c r="B11" s="14">
+        <v>0.14200000000000002</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="14">
+        <v>0.11599999999999999</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>5</v>
-      </c>
-      <c r="C12">
-        <v>0.108</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="14">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="C13">
-        <v>8.2000000000000003E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="14">
+        <v>8.0999999999999989E-2</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>1</v>
-      </c>
-      <c r="C14">
-        <v>8.0999999999999989E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="14">
+        <v>0.08</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="C15">
-        <v>0.08</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="C16">
-        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="14">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>3</v>
-      </c>
-      <c r="C17">
-        <v>6.3E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="14">
+        <v>6.2E-2</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="C18">
-        <v>6.2E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="14">
+        <v>5.3999999999999992E-2</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="C19">
-        <v>5.3999999999999992E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>21</v>
-      </c>
-      <c r="C20">
-        <v>0.05</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="14">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="C21">
-        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="14">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="C22">
-        <v>3.9E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="14">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="C23">
-        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="C24">
-        <v>0.03</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="14">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="C25">
-        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="14">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="C26">
-        <v>0.01</v>
       </c>
     </row>
   </sheetData>
@@ -4517,8 +4582,9 @@
     <sortCondition descending="1" ref="C2:C26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add new mail.ru counter. Add ajax update for chat messages. Signed-off-by:Igor Peshkov <igor.peshkov@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/Rating/Rating.xlsx
+++ b/docs/Rating/Rating.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>Pilots</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Ilya Ivashchenko</t>
+  </si>
+  <si>
+    <t>13-ITA</t>
   </si>
 </sst>
 </file>
@@ -343,14 +346,19 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="60% - Акцент1" xfId="2" builtinId="32"/>
-    <cellStyle name="60% - Акцент5" xfId="5" builtinId="48"/>
-    <cellStyle name="Акцент1" xfId="1" builtinId="29"/>
-    <cellStyle name="Акцент4" xfId="3" builtinId="41"/>
-    <cellStyle name="Акцент5" xfId="4" builtinId="45"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
+    <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Accent4" xfId="3" builtinId="41"/>
+    <cellStyle name="Accent5" xfId="4" builtinId="45"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <i/>
@@ -379,18 +387,18 @@
     <sortCondition descending="1" ref="B1:B27"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Position"/>
-    <tableColumn id="2" name="Rating" dataDxfId="0"/>
-    <tableColumn id="3" name="Pilots" dataDxfId="1"/>
+    <tableColumn id="1" name="Position" dataDxfId="0"/>
+    <tableColumn id="2" name="Rating" dataDxfId="1"/>
+    <tableColumn id="3" name="Pilots" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -428,7 +436,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -500,7 +508,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -676,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AQ32"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="K6" workbookViewId="0">
       <selection activeCell="V5" sqref="V5:W30"/>
     </sheetView>
   </sheetViews>
@@ -739,7 +747,9 @@
       <c r="M3" s="6">
         <v>8</v>
       </c>
-      <c r="N3" s="6"/>
+      <c r="N3" s="6">
+        <v>7</v>
+      </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -788,8 +798,8 @@
       <c r="M4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="8">
-        <v>13</v>
+      <c r="N4" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="O4" s="8">
         <v>14</v>
@@ -866,9 +876,9 @@
         <f t="shared" si="0"/>
         <v>12-Bel</v>
       </c>
-      <c r="AJ4" s="4">
+      <c r="AJ4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>13-ITA</v>
       </c>
       <c r="AK4" s="4">
         <f t="shared" si="0"/>
@@ -1054,7 +1064,9 @@
       <c r="M6" s="9">
         <v>1</v>
       </c>
-      <c r="N6" s="9"/>
+      <c r="N6" s="9">
+        <v>1</v>
+      </c>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
@@ -1064,7 +1076,7 @@
       <c r="U6" s="9"/>
       <c r="V6">
         <f t="shared" si="1"/>
-        <v>0.85399999999999987</v>
+        <v>0.90299999999999991</v>
       </c>
       <c r="W6" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1120,7 +1132,7 @@
       </c>
       <c r="AJ6">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="AK6">
         <f t="shared" si="16"/>
@@ -1290,7 +1302,9 @@
       <c r="M8" s="9">
         <v>2</v>
       </c>
-      <c r="N8" s="9"/>
+      <c r="N8" s="9">
+        <v>2</v>
+      </c>
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
@@ -1300,7 +1314,7 @@
       <c r="U8" s="9"/>
       <c r="V8">
         <f t="shared" si="1"/>
-        <v>0.21799999999999997</v>
+        <v>0.25999999999999995</v>
       </c>
       <c r="W8" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1356,7 +1370,7 @@
       </c>
       <c r="AJ8">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="AK8">
         <f t="shared" si="16"/>
@@ -1540,7 +1554,9 @@
       <c r="M10" s="9">
         <v>5</v>
       </c>
-      <c r="N10" s="9"/>
+      <c r="N10" s="9">
+        <v>3</v>
+      </c>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
@@ -1550,7 +1566,7 @@
       <c r="U10" s="9"/>
       <c r="V10">
         <f t="shared" si="1"/>
-        <v>0.35299999999999998</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="W10" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1606,7 +1622,7 @@
       </c>
       <c r="AJ10">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AK10">
         <f t="shared" si="16"/>
@@ -1798,7 +1814,9 @@
       <c r="M12" s="9">
         <v>4</v>
       </c>
-      <c r="N12" s="9"/>
+      <c r="N12" s="9">
+        <v>5</v>
+      </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
@@ -1808,7 +1826,7 @@
       <c r="U12" s="9"/>
       <c r="V12">
         <f t="shared" si="23"/>
-        <v>0.16600000000000001</v>
+        <v>0.187</v>
       </c>
       <c r="W12" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1864,7 +1882,7 @@
       </c>
       <c r="AJ12">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AK12">
         <f t="shared" si="16"/>
@@ -1931,7 +1949,9 @@
       <c r="M13" s="9">
         <v>6</v>
       </c>
-      <c r="N13" s="9"/>
+      <c r="N13" s="9">
+        <v>4</v>
+      </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
@@ -1941,7 +1961,7 @@
       <c r="U13" s="9"/>
       <c r="V13">
         <f t="shared" si="23"/>
-        <v>0.32800000000000001</v>
+        <v>0.35600000000000004</v>
       </c>
       <c r="W13" s="5" t="str">
         <f t="shared" si="2"/>
@@ -1997,7 +2017,7 @@
       </c>
       <c r="AJ13">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="AK13">
         <f t="shared" si="16"/>
@@ -2411,7 +2431,9 @@
       <c r="M17" s="9">
         <v>3</v>
       </c>
-      <c r="N17" s="9"/>
+      <c r="N17" s="9">
+        <v>6</v>
+      </c>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
@@ -2421,7 +2443,7 @@
       <c r="U17" s="9"/>
       <c r="V17">
         <f t="shared" si="23"/>
-        <v>0.41000000000000003</v>
+        <v>0.42400000000000004</v>
       </c>
       <c r="W17" s="5" t="str">
         <f t="shared" si="2"/>
@@ -2477,7 +2499,7 @@
       </c>
       <c r="AJ17">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AK17">
         <f t="shared" si="16"/>
@@ -3940,7 +3962,9 @@
       <c r="M30" s="9">
         <v>7</v>
       </c>
-      <c r="N30" s="9"/>
+      <c r="N30" s="9">
+        <v>7</v>
+      </c>
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
       <c r="Q30" s="9"/>
@@ -3950,7 +3974,7 @@
       <c r="U30" s="9"/>
       <c r="V30">
         <f t="shared" si="25"/>
-        <v>1.6E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="W30" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4006,7 +4030,7 @@
       </c>
       <c r="AJ30">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AK30">
         <f t="shared" si="16"/>
@@ -4270,7 +4294,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4292,62 +4316,62 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="14">
-        <v>0.85399999999999987</v>
+        <v>0.90299999999999991</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
       <c r="B3" s="14">
-        <v>0.41000000000000003</v>
+        <v>0.42400000000000004</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
       <c r="B4" s="14">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0.35600000000000004</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14">
         <v>0.35599999999999998</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="14">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="14">
-        <v>0.32800000000000001</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
       <c r="B7" s="14">
@@ -4358,7 +4382,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
       <c r="B8" s="14">
@@ -4369,29 +4393,29 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
       <c r="B9" s="14">
-        <v>0.21799999999999997</v>
+        <v>0.25999999999999995</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
       <c r="B10" s="14">
-        <v>0.16600000000000001</v>
+        <v>0.187</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
       <c r="B11" s="14">
@@ -4402,7 +4426,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="13">
         <v>11</v>
       </c>
       <c r="B12" s="14">
@@ -4413,7 +4437,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="13">
         <v>12</v>
       </c>
       <c r="B13" s="14">
@@ -4424,7 +4448,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="13">
         <v>13</v>
       </c>
       <c r="B14" s="14">
@@ -4435,7 +4459,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="13">
         <v>14</v>
       </c>
       <c r="B15" s="14">
@@ -4446,7 +4470,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="13">
         <v>15</v>
       </c>
       <c r="B16" s="14">
@@ -4457,7 +4481,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="13">
         <v>16</v>
       </c>
       <c r="B17" s="14">
@@ -4468,7 +4492,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="13">
         <v>17</v>
       </c>
       <c r="B18" s="14">
@@ -4479,7 +4503,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="13">
         <v>18</v>
       </c>
       <c r="B19" s="14">
@@ -4490,7 +4514,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="13">
         <v>19</v>
       </c>
       <c r="B20" s="14">
@@ -4501,7 +4525,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="13">
         <v>20</v>
       </c>
       <c r="B21" s="14">
@@ -4512,7 +4536,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="13">
         <v>21</v>
       </c>
       <c r="B22" s="14">
@@ -4523,7 +4547,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="13">
         <v>22</v>
       </c>
       <c r="B23" s="14">
@@ -4534,7 +4558,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="13">
         <v>23</v>
       </c>
       <c r="B24" s="14">
@@ -4545,29 +4569,29 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="13">
         <v>24</v>
       </c>
       <c r="B25" s="14">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>25</v>
+      </c>
+      <c r="B26" s="14">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C26" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="14">
-        <v>1.6E-2</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="13">
         <v>26</v>
       </c>
       <c r="B27" s="14">
@@ -4582,7 +4606,7 @@
     <sortCondition descending="1" ref="C2:C26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>